<commit_message>
codigo de escalas antigo está funcionando e adicioinado escala de sonoplastas
</commit_message>
<xml_diff>
--- a/algoritmo_antigo_funcionando/pessoas.xlsx
+++ b/algoritmo_antigo_funcionando/pessoas.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="52">
   <si>
     <t xml:space="preserve">Nome</t>
   </si>
@@ -61,6 +61,9 @@
     <t xml:space="preserve">Tenor</t>
   </si>
   <si>
+    <t xml:space="preserve">quarta</t>
+  </si>
+  <si>
     <t xml:space="preserve">sabado</t>
   </si>
   <si>
@@ -68,9 +71,6 @@
   </si>
   <si>
     <t xml:space="preserve">Mondek</t>
-  </si>
-  <si>
-    <t xml:space="preserve">quarta</t>
   </si>
   <si>
     <t xml:space="preserve">sabado,domingo</t>
@@ -279,7 +279,7 @@
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G27" activeCellId="0" sqref="G27"/>
+      <selection pane="topLeft" activeCell="H19" activeCellId="0" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -337,11 +337,14 @@
       <c r="F2" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="G2" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="H2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>11</v>
@@ -349,7 +352,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>11</v>
@@ -361,7 +364,7 @@
         <v>11</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>17</v>
@@ -444,7 +447,7 @@
         <v>12</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>18</v>
@@ -464,7 +467,7 @@
         <v>12</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>11</v>
@@ -481,7 +484,7 @@
         <v>12</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>26</v>
@@ -501,10 +504,10 @@
         <v>28</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>11</v>
@@ -570,7 +573,7 @@
         <v>11</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>18</v>
@@ -587,10 +590,10 @@
         <v>28</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>18</v>
@@ -610,7 +613,7 @@
         <v>28</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>11</v>
@@ -627,10 +630,10 @@
         <v>11</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -644,10 +647,10 @@
         <v>28</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>11</v>
@@ -701,7 +704,7 @@
         <v>39</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>11</v>
@@ -721,10 +724,10 @@
         <v>11</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>11</v>
@@ -741,10 +744,10 @@
         <v>28</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -758,7 +761,7 @@
         <v>28</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>11</v>
@@ -775,7 +778,7 @@
         <v>28</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>11</v>
@@ -798,7 +801,7 @@
         <v>39</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>11</v>
@@ -815,7 +818,7 @@
         <v>46</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -832,7 +835,7 @@
         <v>46</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>18</v>
@@ -852,7 +855,7 @@
         <v>46</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>18</v>
@@ -875,7 +878,7 @@
         <v>50</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>11</v>
@@ -892,10 +895,10 @@
         <v>46</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>